<commit_message>
Document Excel des cas de Sudoku
</commit_message>
<xml_diff>
--- a/src/sudoku/cas_problèmatiques.xlsx
+++ b/src/sudoku/cas_problèmatiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinrenaud/Code/git-quarto-python/src/sudoku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E42C86-3FCB-D141-B142-256B83A3A9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C7315C-735F-744F-9BC0-CB030CD36200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="520" windowWidth="35840" windowHeight="21900" xr2:uid="{FB6AD995-BC95-DA4B-B1BF-9A67CACA808E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{FB6AD995-BC95-DA4B-B1BF-9A67CACA808E}"/>
   </bookViews>
   <sheets>
     <sheet name="extreme1" sheetId="1" r:id="rId1"/>
@@ -1056,16 +1056,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>26737</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>70584</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>387685</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>137426</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>40106</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>176463</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>401054</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>270041</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1088,7 +1088,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4505158" y="70584"/>
+          <a:off x="6657474" y="2623952"/>
           <a:ext cx="2700422" cy="2592405"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1154,15 +1154,103 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="fr-CA" sz="1100" kern="1200"/>
-            <a:t>Pas de déduction pour N1 et</a:t>
+            <a:t>Pas de déduction pour ni N1,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="fr-CA" sz="1100" kern="1200" baseline="0"/>
-            <a:t> N2</a:t>
+            <a:t> ni N2, ni N3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>169125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33421</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1335</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>367631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{734B4B6F-F9BC-5FBA-FF18-8F7CA9CDF160}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4199704" y="33421"/>
+          <a:ext cx="2519263" cy="3241842"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>6683</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>20052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>426013</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>314158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83089BA-00FD-CC92-D2F8-A626AA125FD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9411367" y="20052"/>
+          <a:ext cx="2210699" cy="5240422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1634,7 +1722,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="32" x14ac:dyDescent="0.2"/>
@@ -1923,7 +2011,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="32" x14ac:dyDescent="0.2"/>

</xml_diff>